<commit_message>
Added some hospitals and rotas
</commit_message>
<xml_diff>
--- a/static/user_input/input_brighton_resp.xlsx
+++ b/static/user_input/input_brighton_resp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vig/Data/Programming/WebDev/F1-rota-converter/static/user_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8896A0-9D4E-9745-B46A-553FFF7C5B82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5F2D98-4C51-3544-8F1D-CAC978BC5B60}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18500" windowHeight="19060" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,42 +663,50 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="22">
@@ -1333,7 +1341,7 @@
   </sheetPr>
   <dimension ref="A1:AG49"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3317,7 +3325,7 @@
   </sheetPr>
   <dimension ref="A1:AF40"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AE26" sqref="AE26"/>
     </sheetView>
   </sheetViews>
@@ -4997,7 +5005,7 @@
   </sheetPr>
   <dimension ref="A1:AG26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="O1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6665,7 +6673,9 @@
   </sheetPr>
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8821,8 +8831,8 @@
   </sheetPr>
   <dimension ref="A1:AG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AG23" sqref="AG23"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>